<commit_message>
saving extraction file as csv and updating full variability metadata file
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
+++ b/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /fullvariability /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C32FF3-EB4E-794C-9B17-3F46E6AF4BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D721294F-97DF-AF47-96B3-14E407397E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="301">
   <si>
     <t>label</t>
   </si>
@@ -847,9 +847,6 @@
   </si>
   <si>
     <t>0306-4565</t>
-  </si>
-  <si>
-    <t>n </t>
   </si>
   <si>
     <t>organismal </t>
@@ -1299,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDF54A4-7244-6B4F-B3C6-F723070AAEF8}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2044,25 +2041,25 @@
     </row>
     <row r="17" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F17" s="2">
         <v>2016</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>20</v>
@@ -2074,10 +2071,10 @@
         <v>21</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>134</v>
@@ -2085,43 +2082,43 @@
     </row>
     <row r="18" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="F18" s="2">
         <v>2016</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="O18" s="2" t="s">
         <v>134</v>
@@ -2407,25 +2404,25 @@
     </row>
     <row r="26" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="F26" s="2">
         <v>2014</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>20</v>
@@ -2440,7 +2437,7 @@
         <v>95</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>134</v>
@@ -2598,7 +2595,7 @@
         <v>21</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>134</v>
@@ -2984,16 +2981,16 @@
         <v>21</v>
       </c>
       <c r="J40" t="s">
-        <v>274</v>
+        <v>21</v>
       </c>
       <c r="K40" t="s">
         <v>56</v>
       </c>
       <c r="L40" t="s">
+        <v>274</v>
+      </c>
+      <c r="M40" t="s">
         <v>275</v>
-      </c>
-      <c r="M40" t="s">
-        <v>276</v>
       </c>
       <c r="N40" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
delnat et al and dong et al extractions and corresponding files
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
+++ b/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /fullvariability /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D721294F-97DF-AF47-96B3-14E407397E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E006EEE-61A2-CF43-8313-21D22D190DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
+    <workbookView xWindow="28800" yWindow="-28000" windowWidth="28800" windowHeight="16060" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="300">
   <si>
     <t>label</t>
   </si>
@@ -825,12 +825,6 @@
     <t>As thermal regimes change worldwide, projections of future population and species persistence often require estimates of how population growth rates depend on temperature. These projections rarely account for how temporal variation in temperature can systematically modify growth rates relative to projections based on constant temperatures. Here, we tested the hypothesis that time-averaged population growth rates in fluctuating thermal environments differ from growth rates in constant conditions as a consequence of Jensen's inequality, and that the thermal performance curves (TPCs) describing population growth in fluctuating environments can be predicted quantitatively based on TPCs generated in constant laboratory conditions. With experimental populations of the green alga Tetraselmis tetrahele, we show that nonlinear averaging techniques accurately predicted increased as well as decreased population growth rates in fluctuating thermal regimes relative to constant thermal regimes. We extrapolate from these results to project critical temperatures for population growth and persistence of 89 phytoplankton species in naturally variable thermal environments. These results advance our ability to predict population dynamics in the context of global change.</t>
   </si>
   <si>
-    <t xml:space="preserve">check supplementary info, constant vs flux </t>
-  </si>
-  <si>
-    <t xml:space="preserve">fig s6 </t>
-  </si>
-  <si>
     <t>Fabricio.Neto_2019_JOOFTHBI</t>
   </si>
   <si>
@@ -882,9 +876,6 @@
     <t>organismal</t>
   </si>
   <si>
-    <t>maybe acclimation</t>
-  </si>
-  <si>
     <t>fig 2,3,5</t>
   </si>
   <si>
@@ -928,6 +919,12 @@
   </si>
   <si>
     <t xml:space="preserve">table 1, fig 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">check supplementary info (figure s6), constant vs flux </t>
+  </si>
+  <si>
+    <t>maybe acclimation; not sure what to do with all these reported genotypes in figure 2-5…considering extracting figure s8</t>
   </si>
 </sst>
 </file>
@@ -943,7 +940,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -962,6 +959,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -975,11 +978,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1296,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDF54A4-7244-6B4F-B3C6-F723070AAEF8}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2039,86 +2043,89 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D17" s="2" t="s">
+    <row r="17" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="F17" s="2">
+      <c r="C17" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" s="4">
         <v>2016</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="O17" s="2" t="s">
+      <c r="G17" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="O17" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="F18" s="2">
         <v>2016</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="L18" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="O18" s="2" t="s">
         <v>134</v>
@@ -2161,6 +2168,9 @@
       <c r="M19" s="2" t="s">
         <v>133</v>
       </c>
+      <c r="N19" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="O19" s="2" t="s">
         <v>134</v>
       </c>
@@ -2202,6 +2212,9 @@
       <c r="M20" s="2" t="s">
         <v>143</v>
       </c>
+      <c r="N20" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="O20" s="2" t="s">
         <v>134</v>
       </c>
@@ -2243,6 +2256,9 @@
       <c r="M21" s="2" t="s">
         <v>158</v>
       </c>
+      <c r="N21" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="O21" s="2" t="s">
         <v>134</v>
       </c>
@@ -2404,25 +2420,25 @@
     </row>
     <row r="26" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="F26" s="2">
         <v>2014</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>20</v>
@@ -2437,7 +2453,7 @@
         <v>95</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>134</v>
@@ -2595,7 +2611,7 @@
         <v>21</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>134</v>
@@ -2939,11 +2955,11 @@
       <c r="J39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>267</v>
+      <c r="K39" t="s">
+        <v>56</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>266</v>
+        <v>298</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>21</v>
@@ -2954,28 +2970,28 @@
     </row>
     <row r="40" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>266</v>
+      </c>
+      <c r="B40" t="s">
+        <v>267</v>
+      </c>
+      <c r="C40" t="s">
         <v>268</v>
-      </c>
-      <c r="B40" t="s">
-        <v>269</v>
-      </c>
-      <c r="C40" t="s">
-        <v>270</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F40">
         <v>2019</v>
       </c>
       <c r="G40" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H40" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I40" t="s">
         <v>21</v>
@@ -2987,10 +3003,10 @@
         <v>56</v>
       </c>
       <c r="L40" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="M40" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="N40" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
saatkamp et al and sheldon et al extractions, files and updates to metafor spreadsheet for fully variability
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
+++ b/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /fullvariability /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E006EEE-61A2-CF43-8313-21D22D190DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA9B38F-31EE-9B43-AE7D-76EF65A14CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-28000" windowWidth="28800" windowHeight="16060" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="294">
   <si>
     <t>label</t>
   </si>
@@ -525,30 +525,6 @@
     <t>unclear, experimental design involves constant acc to flux with an converse trt?</t>
   </si>
   <si>
-    <t>Journal of Insect Physiology</t>
-  </si>
-  <si>
-    <t>Haupt2017108</t>
-  </si>
-  <si>
-    <t>Haupt, T.M. and Sinclair, B.J. and Chown, S.L.</t>
-  </si>
-  <si>
-    <t>Thermal preference and performance in a sub-Antarctic caterpillar: A test of the coadaptation hypothesis and its alternatives</t>
-  </si>
-  <si>
-    <t>10.1016/j.jinsphys.2016.12.006</t>
-  </si>
-  <si>
-    <t>Physiological ecologists have long assumed that thermoregulatory behaviour will evolve to optimise physiological performance. The coadaptation hypothesis predicts that an animal's preferred body temperature will correspond to the temperature at which its performance is optimal. Here we use a strong inference approach to examine the relationship between thermal preference and locomotor performance in the caterpillars of a wingless sub-Antarctic moth, Pringleophaga marioni Viette (Tineidae). The coadaptation hypothesis and its alternatives (suboptimal is optimal, thermodynamic effect, trait variation) are tested. Compared to the optimal movement temperature (22.5C for field-fresh caterpillars and 25, 20, 22.5, 25 and 20C following seven day acclimations to 0, 5, 10, 15 and 515C respectively), caterpillar thermal preference was significantly lower (9.2C for field-fresh individuals and 9.4, 8.8, 8.1, 5.2 and 4.6C following acclimation to 0, 5, 10, 15 and 515C, respectively). Together with the low degree of asymmetry observed in the performance curves, and the finding that acclimation to high temperatures did not result in maximal performance, all, but one of the above hypotheses (i.e. trait variation) was rejected. The thermal preference of P. marioni caterpillars more closely resembles temperatures at which survival is high (510C), or where feeding is optimal (10C), than where locomotion speed is maximal, suggesting that thermal preference may be optimised for overall fitness rather than for a given trait.  2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">table 1a, 2 </t>
-  </si>
-  <si>
-    <t>acclimation….maybe also included in the full analysis</t>
-  </si>
-  <si>
     <t>Imholt2011436</t>
   </si>
   <si>
@@ -925,6 +901,12 @@
   </si>
   <si>
     <t>maybe acclimation; not sure what to do with all these reported genotypes in figure 2-5…considering extracting figure s8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">had to convert 95%CI to SD </t>
+  </si>
+  <si>
+    <t>only extracted end weights to avoid colinearity of time series data; study used multiple age stages so I just coded as adults since they were held in captivity for a while?</t>
   </si>
 </sst>
 </file>
@@ -1298,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDF54A4-7244-6B4F-B3C6-F723070AAEF8}">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2045,25 +2027,25 @@
     </row>
     <row r="17" spans="1:15" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F17" s="4">
         <v>2016</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>20</v>
@@ -2075,10 +2057,10 @@
         <v>21</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>134</v>
@@ -2086,25 +2068,25 @@
     </row>
     <row r="18" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="F18" s="2">
         <v>2016</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>20</v>
@@ -2116,13 +2098,13 @@
         <v>21</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>21</v>
@@ -2263,69 +2245,66 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F22" s="2">
-        <v>2017</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="M22" s="2" t="s">
+    <row r="22" spans="1:15" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="B22" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2013</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O22" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2">
+        <v>2015</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F23" s="2">
-        <v>2013</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="H23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2336,7 +2315,13 @@
         <v>21</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>186</v>
+        <v>38</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>134</v>
@@ -2344,26 +2329,26 @@
     </row>
     <row r="24" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="F24" s="2">
+        <v>2010</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2015</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="H24" s="2" t="s">
         <v>20</v>
       </c>
@@ -2374,33 +2359,39 @@
         <v>21</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="O24" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>193</v>
+        <v>282</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>194</v>
+        <v>283</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>195</v>
+        <v>284</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>196</v>
+        <v>285</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>197</v>
+        <v>286</v>
       </c>
       <c r="F25" s="2">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>198</v>
+        <v>287</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>20</v>
@@ -2412,86 +2403,95 @@
         <v>21</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F26" s="2">
-        <v>2014</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="O26" s="2" t="s">
+    <row r="26" spans="1:15" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F26" s="4">
+        <v>2021</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="O26" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2">
+        <v>2011</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F27" s="2">
-        <v>2021</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>204</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>134</v>
@@ -2499,25 +2499,25 @@
     </row>
     <row r="28" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>208</v>
+        <v>162</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="F28" s="2">
-        <v>2011</v>
+        <v>2020</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>20</v>
@@ -2529,10 +2529,13 @@
         <v>21</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>212</v>
+        <v>219</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>134</v>
@@ -2540,25 +2543,25 @@
     </row>
     <row r="29" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>162</v>
+        <v>229</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F29" s="2">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>20</v>
@@ -2570,10 +2573,7 @@
         <v>21</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>227</v>
+        <v>289</v>
       </c>
       <c r="O29" s="2" t="s">
         <v>134</v>
@@ -2581,101 +2581,101 @@
     </row>
     <row r="30" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="H30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="F30" s="2">
-        <v>2009</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="F31" s="2">
-        <v>2020</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="O31" s="2" t="s">
+    <row r="31" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F31" s="3">
+        <v>2005</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O31" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="F32" s="3">
-        <v>2005</v>
+        <v>2019</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>20</v>
@@ -2687,7 +2687,7 @@
         <v>135</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="O32" s="3" t="s">
         <v>134</v>
@@ -2695,25 +2695,25 @@
     </row>
     <row r="33" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="F33" s="3">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>20</v>
@@ -2725,7 +2725,7 @@
         <v>135</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="O33" s="3" t="s">
         <v>134</v>
@@ -2733,25 +2733,25 @@
     </row>
     <row r="34" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="F34" s="3">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>20</v>
@@ -2762,8 +2762,11 @@
       <c r="J34" s="3" t="s">
         <v>135</v>
       </c>
+      <c r="K34" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="M34" s="3" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="O34" s="3" t="s">
         <v>134</v>
@@ -2771,25 +2774,25 @@
     </row>
     <row r="35" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="F35" s="3">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>20</v>
@@ -2800,37 +2803,31 @@
       <c r="J35" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="O35" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="F36" s="3">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>20</v>
@@ -2841,31 +2838,37 @@
       <c r="J36" s="3" t="s">
         <v>135</v>
       </c>
+      <c r="K36" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="O36" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="F37" s="3">
+        <v>2018</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="F37" s="3">
-        <v>2020</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>20</v>
@@ -2876,149 +2879,108 @@
       <c r="J37" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>204</v>
-      </c>
       <c r="M37" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O37" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:15" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="D38" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="E38" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="F38" s="3">
-        <v>2018</v>
-      </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>258</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="M38" s="3" t="s">
+      <c r="B39" t="s">
         <v>259</v>
       </c>
-      <c r="O38" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="C39" t="s">
         <v>260</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
         <v>261</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="F39">
+        <v>2019</v>
+      </c>
+      <c r="G39" t="s">
         <v>262</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="H39" t="s">
         <v>263</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F39" s="1">
-        <v>2018</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>22</v>
+      <c r="I39" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" t="s">
+        <v>21</v>
       </c>
       <c r="K39" t="s">
         <v>56</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="N39" s="1" t="s">
+      <c r="L39" t="s">
+        <v>264</v>
+      </c>
+      <c r="M39" t="s">
+        <v>265</v>
+      </c>
+      <c r="N39" t="s">
         <v>21</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>266</v>
-      </c>
-      <c r="B40" t="s">
-        <v>267</v>
-      </c>
-      <c r="C40" t="s">
-        <v>268</v>
-      </c>
-      <c r="D40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" t="s">
-        <v>269</v>
-      </c>
-      <c r="F40">
-        <v>2019</v>
-      </c>
-      <c r="G40" t="s">
-        <v>270</v>
-      </c>
-      <c r="H40" t="s">
-        <v>271</v>
-      </c>
-      <c r="I40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J40" t="s">
-        <v>21</v>
-      </c>
-      <c r="K40" t="s">
-        <v>56</v>
-      </c>
-      <c r="L40" t="s">
-        <v>272</v>
-      </c>
-      <c r="M40" t="s">
-        <v>273</v>
-      </c>
-      <c r="N40" t="s">
-        <v>21</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T38">
-    <sortCondition descending="1" ref="O2:O38"/>
-    <sortCondition descending="1" ref="J2:J38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T37">
+    <sortCondition descending="1" ref="O2:O37"/>
+    <sortCondition descending="1" ref="J2:J37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
comitting partial completion of verheyen extraction
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
+++ b/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /fullvariability /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA9B38F-31EE-9B43-AE7D-76EF65A14CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85975A1-9367-0E41-B4EE-EB1980497FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-28000" windowWidth="28800" windowHeight="16060" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="296">
   <si>
     <t>label</t>
   </si>
@@ -907,6 +907,12 @@
   </si>
   <si>
     <t>only extracted end weights to avoid colinearity of time series data; study used multiple age stages so I just coded as adults since they were held in captivity for a while?</t>
+  </si>
+  <si>
+    <t>no reported error on figure 1, excluded</t>
+  </si>
+  <si>
+    <t>assumed lower sample size range of 24 (range = 24-26)</t>
   </si>
 </sst>
 </file>
@@ -1282,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDF54A4-7244-6B4F-B3C6-F723070AAEF8}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2575,6 +2581,12 @@
       <c r="K29" s="2" t="s">
         <v>289</v>
       </c>
+      <c r="M29" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="O29" s="2" t="s">
         <v>134</v>
       </c>
@@ -2612,6 +2624,12 @@
       </c>
       <c r="K30" s="2" t="s">
         <v>238</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
updates to full variability metadata
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
+++ b/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /fullvariability /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34451876-3827-EF45-854E-BB497FA8B53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4822F2-DBDE-0341-9821-E7006D3A2921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-28000" windowWidth="24000" windowHeight="16060" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
+    <workbookView xWindow="28800" yWindow="-16440" windowWidth="24000" windowHeight="13620" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDF54A4-7244-6B4F-B3C6-F723070AAEF8}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2837,82 +2837,82 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:15" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="4">
         <v>2020</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="3" t="s">
+      <c r="H36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="K36" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="M36" s="3" t="s">
+      <c r="M36" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="O36" s="3" t="s">
+      <c r="O36" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:15" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="4">
         <v>2018</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J37" s="3" t="s">
+      <c r="H37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="M37" s="3" t="s">
+      <c r="M37" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="O37" s="3" t="s">
+      <c r="O37" s="4" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prakoso et al extraction
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
+++ b/data extraction /lit search metadata /fullvariability /fullvariability_7jun21.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /fullvariability /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFAB159-FC50-884F-AC4B-4749CD16165D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AD9435-3948-8B46-8FA9-6FD65D985835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28780" yWindow="-14600" windowWidth="24000" windowHeight="13620" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
+    <workbookView xWindow="2100" yWindow="460" windowWidth="24000" windowHeight="13620" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$P$40</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="313">
   <si>
     <t>label</t>
   </si>
@@ -961,6 +964,9 @@
   </si>
   <si>
     <t>excluded some treatments because non-normally distributed data; excluded 25 C treatment and 30 C</t>
+  </si>
+  <si>
+    <t>didn't extract figure 5 as nothing reported for flux trt</t>
   </si>
 </sst>
 </file>
@@ -976,7 +982,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -985,19 +991,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,12 +1008,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,1806 +1328,1819 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDF54A4-7244-6B4F-B3C6-F723070AAEF8}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>2009</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>2011</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="N3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>2019</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="N4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>2015</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="N5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>2014</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="N6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>2018</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="N7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>2019</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="N8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>2015</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="N9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="N9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>2016</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="N10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>2012</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="H11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="N11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="N11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="1" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>2014</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="N12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>2007</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N13" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="N13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>2016</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="N14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="N14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>2004</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="H15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="N15" t="s">
-        <v>21</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="N15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>2018</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="N16" t="s">
-        <v>21</v>
-      </c>
-      <c r="O16" t="s">
+      <c r="N16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C19" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D19" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E19" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F19" s="1">
         <v>2016</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G19" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="4" t="s">
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M19" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="O17" s="4" t="s">
+      <c r="N19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F20" s="1">
         <v>2016</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="2" t="s">
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L20" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M20" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O18" s="2" t="s">
+      <c r="N20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F21" s="1">
         <v>2012</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" s="2" t="s">
+      <c r="N21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F22" s="1">
         <v>2019</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="2" t="s">
+      <c r="H22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O20" s="2" t="s">
+      <c r="N22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F23" s="1">
         <v>2008</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="2" t="s">
+      <c r="H23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M23" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O21" s="2" t="s">
+      <c r="N23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F22" s="3">
-        <v>2013</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="O22" s="3" t="s">
+    <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2015</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2015</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="2" t="s">
+    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2010</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2010</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O24" s="2" t="s">
+    <row r="26" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2014</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F25" s="2">
-        <v>2014</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O25" s="2" t="s">
+    <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="F26" s="4">
-        <v>2021</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="O26" s="4" t="s">
+    <row r="28" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2009</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F27" s="3">
-        <v>2011</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F28" s="3">
+    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F29" s="1">
         <v>2020</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F29" s="2">
-        <v>2009</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O29" s="2" t="s">
+      <c r="G29" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>228</v>
+        <v>301</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>229</v>
+        <v>302</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>231</v>
+        <v>304</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>232</v>
+        <v>305</v>
       </c>
       <c r="F30" s="2">
         <v>2020</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>233</v>
+        <v>306</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>20</v>
+        <v>307</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>234</v>
+        <v>287</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>21</v>
+        <v>287</v>
       </c>
       <c r="O30" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="2">
+        <v>2013</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="O31" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F32" s="2">
+        <v>2011</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F33" s="2">
+        <v>2020</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F34" s="2">
         <v>2005</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="3" t="s">
+      <c r="H34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M34" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="N31" s="3" t="s">
+      <c r="N34" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O34" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="35" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F35" s="2">
         <v>2019</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J32" s="3" t="s">
+      <c r="H35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="M35" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="N32" s="3" t="s">
+      <c r="N35" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O32" s="3" t="s">
+      <c r="O35" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="36" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F36" s="2">
         <v>2011</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" s="3" t="s">
+      <c r="H36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M33" s="3" t="s">
+      <c r="M36" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="N33" s="3" t="s">
+      <c r="N36" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O33" s="3" t="s">
+      <c r="O36" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="37" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F37" s="2">
         <v>2016</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="3" t="s">
+      <c r="H37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K37" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="M34" s="3" t="s">
+      <c r="M37" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="N34" s="3" t="s">
+      <c r="N37" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O34" s="3" t="s">
+      <c r="O37" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="38" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F38" s="2">
         <v>2018</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" s="3" t="s">
+      <c r="H38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M35" s="3" t="s">
+      <c r="M38" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="N35" s="3" t="s">
+      <c r="N38" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O35" s="3" t="s">
+      <c r="O38" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="39" spans="1:16" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F39" s="2">
         <v>2020</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="3" t="s">
+      <c r="H39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="K39" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="M36" s="3" t="s">
+      <c r="M39" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="N36" s="3" t="s">
+      <c r="N39" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O36" s="3" t="s">
+      <c r="O39" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="40" spans="1:16" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F40" s="2">
         <v>2018</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J37" s="3" t="s">
+      <c r="H40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M37" s="3" t="s">
+      <c r="M40" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="N37" s="3" t="s">
+      <c r="N40" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="O37" s="3" t="s">
+      <c r="O40" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F38" s="1">
-        <v>2018</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K38" t="s">
-        <v>56</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>252</v>
-      </c>
-      <c r="B39" t="s">
-        <v>253</v>
-      </c>
-      <c r="C39" t="s">
-        <v>254</v>
-      </c>
-      <c r="D39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" t="s">
-        <v>255</v>
-      </c>
-      <c r="F39">
-        <v>2019</v>
-      </c>
-      <c r="G39" t="s">
-        <v>256</v>
-      </c>
-      <c r="H39" t="s">
-        <v>257</v>
-      </c>
-      <c r="I39" t="s">
-        <v>21</v>
-      </c>
-      <c r="J39" t="s">
-        <v>21</v>
-      </c>
-      <c r="K39" t="s">
-        <v>56</v>
-      </c>
-      <c r="L39" t="s">
-        <v>258</v>
-      </c>
-      <c r="M39" t="s">
-        <v>259</v>
-      </c>
-      <c r="N39" t="s">
-        <v>21</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="F40" s="3">
-        <v>2020</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="O40" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T37">
-    <sortCondition descending="1" ref="O2:O37"/>
-    <sortCondition descending="1" ref="J2:J37"/>
+  <autoFilter ref="A2:P40" xr:uid="{244CEB28-D3C0-EB47-818A-21E7D507A851}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P42">
+    <sortCondition descending="1" ref="N2:N42"/>
+    <sortCondition descending="1" ref="O2:O42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>